<commit_message>
Code Working - Commerce, ED and DD. But not for Util.
</commit_message>
<xml_diff>
--- a/migrate3 - Copy.xlsx
+++ b/migrate3 - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/nilesh_thakur_accenture_com/Documents/Whitepaper/ExcelToAPI2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\ExcelToAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{DFE47717-DE4A-4B65-8462-E9E832AB4E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C613836C-A389-4314-B361-910FB3B0C0C7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF968291-F2ED-4072-AD02-908C9CF31794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0A95F42-B9FA-4697-81E7-8A75D2048534}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="55">
   <si>
     <t>resourceType</t>
   </si>
@@ -137,7 +137,70 @@
     <t>attribute</t>
   </si>
   <si>
-    <t>AutoT2</t>
+    <t>Constraint Margin Rate based on  Add Tax</t>
+  </si>
+  <si>
+    <t>marginRateBasedOnFreightAndAddTax</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>Test_SR</t>
+  </si>
+  <si>
+    <t>test_SR</t>
+  </si>
+  <si>
+    <t>library</t>
+  </si>
+  <si>
+    <t>Tax Exempt Reason</t>
+  </si>
+  <si>
+    <t>taxExemptReason</t>
+  </si>
+  <si>
+    <t>User Import</t>
+  </si>
+  <si>
+    <t>oRCL_SFDC_UserImport</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>Demo28AugT1</t>
+  </si>
+  <si>
+    <t>Document Designer</t>
+  </si>
+  <si>
+    <t>DOCUMENT_DESIGNER</t>
+  </si>
+  <si>
+    <t>_set</t>
+  </si>
+  <si>
+    <t>Field Profile Sheet - English</t>
+  </si>
+  <si>
+    <t>doc_designer</t>
+  </si>
+  <si>
+    <t>Job Profile Sheet - English</t>
+  </si>
+  <si>
+    <t>Email Designer</t>
+  </si>
+  <si>
+    <t>EMAIL_DESIGNER</t>
+  </si>
+  <si>
+    <t>Final Approval Notification For DOA - English</t>
+  </si>
+  <si>
+    <t>email_designer</t>
   </si>
 </sst>
 </file>
@@ -530,9 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991D8937-EF2D-4E7C-A283-A813F0E97320}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -592,7 +657,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -618,17 +683,15 @@
       <c r="I2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="J2" s="5"/>
       <c r="K2" s="3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -660,13 +723,13 @@
         <v>17</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -689,22 +752,22 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -727,22 +790,256 @@
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>